<commit_message>
Updated process format, zip file with create prototype
</commit_message>
<xml_diff>
--- a/src/dist/templates/Format.xlsx
+++ b/src/dist/templates/Format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>required|min:3|max:256</t>
-  </si>
-  <si>
     <t>PostId</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>Posts</t>
+  </si>
+  <si>
+    <t>required|minlength:3|maxlength:256</t>
   </si>
 </sst>
 </file>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,15 +550,15 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,7 +591,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,7 +602,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -645,7 +645,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -671,7 +673,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -682,18 +684,18 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -704,7 +706,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -715,7 +717,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -739,22 +741,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated process: ignore headers empty
</commit_message>
<xml_diff>
--- a/src/dist/templates/Format.xlsx
+++ b/src/dist/templates/Format.xlsx
@@ -125,6 +125,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,9 +186,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,10 +647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D1" sqref="D1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +658,7 @@
     <col min="1" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,7 +669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -675,8 +679,9 @@
       <c r="C2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -686,8 +691,9 @@
       <c r="C3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -698,7 +704,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -709,7 +715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -719,6 +725,13 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Updated process format: ignored sheet when names starts with _ (underscore)
</commit_message>
<xml_diff>
--- a/src/dist/templates/Format.xlsx
+++ b/src/dist/templates/Format.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="1" r:id="rId1"/>
     <sheet name="Comments" sheetId="2" r:id="rId2"/>
-    <sheet name="HiddenSheetTest" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="_Ignored" sheetId="4" r:id="rId3"/>
+    <sheet name="HiddenSheetTest" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -649,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,6 +741,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fixed names: singularize and pluralize
</commit_message>
<xml_diff>
--- a/src/dist/templates/Format.xlsx
+++ b/src/dist/templates/Format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="1" r:id="rId1"/>
@@ -113,13 +113,13 @@
     <t>pk|ai|required</t>
   </si>
   <si>
-    <t>required|fk:posts,title</t>
-  </si>
-  <si>
     <t>Posts</t>
   </si>
   <si>
     <t>required|minlength:3|maxlength:256</t>
+  </si>
+  <si>
+    <t>required|fk:Posts,title</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +690,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -702,7 +702,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -744,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Updated template with actions and language example
</commit_message>
<xml_diff>
--- a/src/dist/templates/Format.xlsx
+++ b/src/dist/templates/Format.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24110"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\var\www\flexphp\flex-generator\src\dist\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA993AB7-3DDE-4158-84DF-E90DA6BF85D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="1" r:id="rId1"/>
     <sheet name="Comments" sheetId="2" r:id="rId2"/>
-    <sheet name="_Ignored" sheetId="4" r:id="rId3"/>
-    <sheet name="HiddenSheetTest" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="Actions" sheetId="5" r:id="rId3"/>
+    <sheet name="_Ignored" sheetId="4" r:id="rId4"/>
+    <sheet name="HiddenSheetTest" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -27,7 +38,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Posts</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>fas fa-mail</t>
+  </si>
   <si>
     <t>Name</t>
   </si>
@@ -44,18 +67,24 @@
     <t>integer</t>
   </si>
   <si>
-    <t>Title</t>
+    <t>pk|ai|required|type:number</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
+    <t>required|maxlength:255</t>
+  </si>
+  <si>
     <t>Content</t>
   </si>
   <si>
     <t>text</t>
   </si>
   <si>
+    <t>required|type:textarea|length:10,512</t>
+  </si>
+  <si>
     <t>IsActive</t>
   </si>
   <si>
@@ -68,15 +97,45 @@
     <t>datetime</t>
   </si>
   <si>
+    <t>ca</t>
+  </si>
+  <si>
     <t>UpdatedAt</t>
   </si>
   <si>
+    <t>ua</t>
+  </si>
+  <si>
+    <t>pk|ai|required</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
+    <t>required|minlength:3|maxlength:256</t>
+  </si>
+  <si>
     <t>PostId</t>
   </si>
   <si>
+    <t>required|fk:Posts,title</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>icf</t>
+  </si>
+  <si>
+    <t>minlength:3|maxlength:256</t>
+  </si>
+  <si>
     <t>Hiidden</t>
   </si>
   <si>
@@ -87,49 +146,16 @@
   </si>
   <si>
     <t>Ignored</t>
-  </si>
-  <si>
-    <t>pk|ai|required|type:number</t>
-  </si>
-  <si>
-    <t>required|maxlength:255</t>
-  </si>
-  <si>
-    <t>required|type:textarea|length:10,512</t>
-  </si>
-  <si>
-    <t>ca</t>
-  </si>
-  <si>
-    <t>ua</t>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>fas fa-mail</t>
-  </si>
-  <si>
-    <t>pk|ai|required</t>
-  </si>
-  <si>
-    <t>Posts</t>
-  </si>
-  <si>
-    <t>required|minlength:3|maxlength:256</t>
-  </si>
-  <si>
-    <t>required|fk:Posts,title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -538,106 +564,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -647,91 +673,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="G8" s="2"/>
     </row>
   </sheetData>
@@ -741,48 +767,127 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD2EC28-BF6C-471B-BEB7-7DC0BF4E349A}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1025" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="G10" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>